<commit_message>
updates of data and text
</commit_message>
<xml_diff>
--- a/analysis/data/derived_data/QSY_lithic_assemblage.xlsx
+++ b/analysis/data/derived_data/QSY_lithic_assemblage.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Lithic_Analysis\QSYSpheroidsStudy\analysis\data\derived_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8FA750A-7EFF-40CC-B6A4-46E5D0E30FE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F54BB2C5-BAA1-48A6-9926-E385AE92F371}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{AB97B327-3DD6-4E43-82ED-5E3E3CC8E6BE}"/>
   </bookViews>
@@ -279,14 +279,8 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -313,17 +307,14 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="176" fontId="7" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -332,10 +323,10 @@
     <xf numFmtId="176" fontId="7" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="176" fontId="10" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -343,6 +334,15 @@
     </xf>
     <xf numFmtId="176" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -666,362 +666,362 @@
   <dimension ref="A1:L14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="16384" width="8.88671875" style="4"/>
+    <col min="1" max="16384" width="8.88671875" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
-      <c r="C1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2" t="s">
+      <c r="C1" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2" t="s">
+      <c r="F1" s="25"/>
+      <c r="G1" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2" t="s">
+      <c r="H1" s="25"/>
+      <c r="I1" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="J1" s="2"/>
-      <c r="K1" s="3" t="s">
+      <c r="J1" s="25"/>
+      <c r="K1" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="L1" s="3"/>
+      <c r="L1" s="26"/>
     </row>
     <row r="2" spans="1:12" ht="15">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="I2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="J2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="K2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="L2" s="5" t="s">
+      <c r="L2" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="15">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="1"/>
-      <c r="C3" s="7">
+      <c r="C3" s="5">
         <f>C4+C5+C6+C7</f>
         <v>177</v>
       </c>
-      <c r="D3" s="8">
+      <c r="D3" s="6">
         <f>C3/636</f>
         <v>0.27830188679245282</v>
       </c>
-      <c r="E3" s="7">
+      <c r="E3" s="5">
         <f>E4+E5+E6+E7</f>
         <v>65</v>
       </c>
-      <c r="F3" s="8">
+      <c r="F3" s="6">
         <f>E3/271</f>
         <v>0.23985239852398524</v>
       </c>
-      <c r="G3" s="7">
+      <c r="G3" s="5">
         <f>+G4+G5+G6+G7</f>
         <v>4</v>
       </c>
-      <c r="H3" s="8">
+      <c r="H3" s="6">
         <f>G3/29</f>
         <v>0.13793103448275862</v>
       </c>
-      <c r="I3" s="7">
+      <c r="I3" s="5">
         <f>I4+I5+I6+I7</f>
         <v>2</v>
       </c>
-      <c r="J3" s="9">
+      <c r="J3" s="7">
         <f>I3/18</f>
         <v>0.1111111111111111</v>
       </c>
-      <c r="K3" s="10">
+      <c r="K3" s="8">
         <f>C3+E3+G3+I3</f>
         <v>248</v>
       </c>
-      <c r="L3" s="9">
-        <f>K3/954</f>
-        <v>0.25995807127882598</v>
+      <c r="L3" s="7">
+        <f>K3/955</f>
+        <v>0.25968586387434556</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="15">
-      <c r="A4" s="6"/>
-      <c r="B4" s="6" t="s">
+      <c r="A4" s="4"/>
+      <c r="B4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="15">
+      <c r="C4" s="13">
         <v>66</v>
       </c>
-      <c r="D4" s="11">
+      <c r="D4" s="9">
         <f t="shared" ref="D4:D11" si="0">C4/637</f>
         <v>0.10361067503924647</v>
       </c>
-      <c r="E4" s="15">
-        <v>24</v>
-      </c>
-      <c r="F4" s="11">
+      <c r="E4" s="13">
+        <v>23</v>
+      </c>
+      <c r="F4" s="9">
         <f t="shared" ref="F4:F13" si="1">E4/271</f>
-        <v>8.8560885608856083E-2</v>
-      </c>
-      <c r="G4" s="15">
+        <v>8.4870848708487087E-2</v>
+      </c>
+      <c r="G4" s="13">
         <v>3</v>
       </c>
-      <c r="H4" s="11">
+      <c r="H4" s="9">
         <f t="shared" ref="H4:H13" si="2">G4/29</f>
         <v>0.10344827586206896</v>
       </c>
-      <c r="I4" s="15">
+      <c r="I4" s="13">
         <v>1</v>
       </c>
-      <c r="J4" s="12">
+      <c r="J4" s="10">
         <f t="shared" ref="J4:J13" si="3">I4/20</f>
         <v>0.05</v>
       </c>
-      <c r="K4" s="13">
+      <c r="K4" s="11">
         <f t="shared" ref="K4:K14" si="4">C4+E4+G4+I4</f>
-        <v>94</v>
-      </c>
-      <c r="L4" s="14">
+        <v>93</v>
+      </c>
+      <c r="L4" s="12">
         <f t="shared" ref="L4:L11" si="5">K4/957</f>
-        <v>9.8223615464994779E-2</v>
+        <v>9.7178683385579931E-2</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="15">
-      <c r="A5" s="6"/>
+      <c r="A5" s="4"/>
       <c r="B5" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C5" s="15">
+      <c r="C5" s="13">
         <v>10</v>
       </c>
-      <c r="D5" s="11">
+      <c r="D5" s="9">
         <f t="shared" si="0"/>
         <v>1.5698587127158554E-2</v>
       </c>
-      <c r="E5" s="15">
-        <v>2</v>
-      </c>
-      <c r="F5" s="11">
+      <c r="E5" s="13">
+        <v>3</v>
+      </c>
+      <c r="F5" s="9">
         <f t="shared" si="1"/>
-        <v>7.3800738007380072E-3</v>
+        <v>1.107011070110701E-2</v>
       </c>
       <c r="G5" s="1">
         <v>0</v>
       </c>
-      <c r="H5" s="11">
+      <c r="H5" s="9">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="I5" s="1">
         <v>0</v>
       </c>
-      <c r="J5" s="12">
+      <c r="J5" s="10">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="K5" s="13">
+      <c r="K5" s="11">
         <f t="shared" si="4"/>
-        <v>12</v>
-      </c>
-      <c r="L5" s="14">
+        <v>13</v>
+      </c>
+      <c r="L5" s="12">
         <f t="shared" si="5"/>
-        <v>1.2539184952978056E-2</v>
+        <v>1.3584117032392894E-2</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="15">
       <c r="A6" s="1"/>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="15">
+      <c r="C6" s="13">
         <v>49</v>
       </c>
-      <c r="D6" s="11">
+      <c r="D6" s="9">
         <f t="shared" si="0"/>
         <v>7.6923076923076927E-2</v>
       </c>
-      <c r="E6" s="15">
+      <c r="E6" s="13">
         <v>11</v>
       </c>
-      <c r="F6" s="11">
+      <c r="F6" s="9">
         <f t="shared" si="1"/>
         <v>4.0590405904059039E-2</v>
       </c>
       <c r="G6" s="1">
         <v>0</v>
       </c>
-      <c r="H6" s="11">
+      <c r="H6" s="9">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="I6" s="1">
         <v>0</v>
       </c>
-      <c r="J6" s="12">
+      <c r="J6" s="10">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="K6" s="13">
+      <c r="K6" s="11">
         <f t="shared" si="4"/>
         <v>60</v>
       </c>
-      <c r="L6" s="14">
+      <c r="L6" s="12">
         <f t="shared" si="5"/>
         <v>6.2695924764890276E-2</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="15">
       <c r="A7" s="1"/>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="15">
+      <c r="C7" s="13">
         <v>52</v>
       </c>
-      <c r="D7" s="11">
+      <c r="D7" s="9">
         <f t="shared" si="0"/>
         <v>8.1632653061224483E-2</v>
       </c>
-      <c r="E7" s="15">
+      <c r="E7" s="13">
         <v>28</v>
       </c>
-      <c r="F7" s="11">
+      <c r="F7" s="9">
         <f t="shared" si="1"/>
         <v>0.10332103321033211</v>
       </c>
-      <c r="G7" s="15">
+      <c r="G7" s="13">
         <v>1</v>
       </c>
-      <c r="H7" s="11">
+      <c r="H7" s="9">
         <f t="shared" si="2"/>
         <v>3.4482758620689655E-2</v>
       </c>
-      <c r="I7" s="15">
+      <c r="I7" s="13">
         <v>1</v>
       </c>
-      <c r="J7" s="12">
+      <c r="J7" s="10">
         <f t="shared" si="3"/>
         <v>0.05</v>
       </c>
-      <c r="K7" s="13">
+      <c r="K7" s="11">
         <f t="shared" si="4"/>
         <v>82</v>
       </c>
-      <c r="L7" s="14">
+      <c r="L7" s="12">
         <f t="shared" si="5"/>
         <v>8.5684430512016713E-2</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="15">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="6"/>
-      <c r="C8" s="10">
+      <c r="B8" s="4"/>
+      <c r="C8" s="8">
         <f>+C9+C10+C11</f>
         <v>450</v>
       </c>
-      <c r="D8" s="8">
+      <c r="D8" s="6">
         <f>C8/636</f>
         <v>0.70754716981132071</v>
       </c>
-      <c r="E8" s="10">
+      <c r="E8" s="8">
         <f>E9+E10+E11</f>
         <v>199</v>
       </c>
-      <c r="F8" s="8">
+      <c r="F8" s="6">
         <f t="shared" si="1"/>
         <v>0.73431734317343178</v>
       </c>
-      <c r="G8" s="10">
+      <c r="G8" s="8">
         <f>G9+G10+G11</f>
         <v>21</v>
       </c>
-      <c r="H8" s="8">
+      <c r="H8" s="6">
         <f t="shared" si="2"/>
         <v>0.72413793103448276</v>
       </c>
-      <c r="I8" s="10">
+      <c r="I8" s="8">
         <f>I9+I10+I11</f>
         <v>16</v>
       </c>
-      <c r="J8" s="9">
+      <c r="J8" s="7">
         <f>I8/18</f>
         <v>0.88888888888888884</v>
       </c>
-      <c r="K8" s="10">
+      <c r="K8" s="8">
         <f t="shared" si="4"/>
         <v>686</v>
       </c>
-      <c r="L8" s="9">
-        <f>K8/954</f>
-        <v>0.7190775681341719</v>
+      <c r="L8" s="7">
+        <f>K8/955</f>
+        <v>0.71832460732984293</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="15">
-      <c r="A9" s="6"/>
-      <c r="B9" s="6" t="s">
+      <c r="A9" s="4"/>
+      <c r="B9" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="15">
+      <c r="C9" s="13">
         <v>224</v>
       </c>
-      <c r="D9" s="11">
+      <c r="D9" s="9">
         <f t="shared" si="0"/>
         <v>0.35164835164835168</v>
       </c>
-      <c r="E9" s="15">
+      <c r="E9" s="13">
         <v>107</v>
       </c>
-      <c r="F9" s="11">
+      <c r="F9" s="9">
         <f t="shared" si="1"/>
         <v>0.39483394833948338</v>
       </c>
-      <c r="G9" s="15">
+      <c r="G9" s="13">
         <v>8</v>
       </c>
-      <c r="H9" s="11">
+      <c r="H9" s="9">
         <f t="shared" si="2"/>
         <v>0.27586206896551724</v>
       </c>
-      <c r="I9" s="15">
+      <c r="I9" s="13">
         <v>5</v>
       </c>
-      <c r="J9" s="12">
+      <c r="J9" s="10">
         <f t="shared" si="3"/>
         <v>0.25</v>
       </c>
@@ -1029,41 +1029,41 @@
         <f t="shared" si="4"/>
         <v>344</v>
       </c>
-      <c r="L9" s="12">
+      <c r="L9" s="10">
         <f t="shared" si="5"/>
         <v>0.35945663531870431</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="15">
       <c r="A10" s="1"/>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="15">
+      <c r="C10" s="13">
         <v>122</v>
       </c>
-      <c r="D10" s="11">
+      <c r="D10" s="9">
         <f t="shared" si="0"/>
         <v>0.19152276295133439</v>
       </c>
-      <c r="E10" s="15">
+      <c r="E10" s="13">
         <v>52</v>
       </c>
-      <c r="F10" s="11">
+      <c r="F10" s="9">
         <f t="shared" si="1"/>
         <v>0.1918819188191882</v>
       </c>
-      <c r="G10" s="15">
+      <c r="G10" s="13">
         <v>9</v>
       </c>
-      <c r="H10" s="11">
+      <c r="H10" s="9">
         <f t="shared" si="2"/>
         <v>0.31034482758620691</v>
       </c>
-      <c r="I10" s="15">
+      <c r="I10" s="13">
         <v>8</v>
       </c>
-      <c r="J10" s="12">
+      <c r="J10" s="10">
         <f t="shared" si="3"/>
         <v>0.4</v>
       </c>
@@ -1071,41 +1071,41 @@
         <f t="shared" si="4"/>
         <v>191</v>
       </c>
-      <c r="L10" s="12">
+      <c r="L10" s="10">
         <f t="shared" si="5"/>
         <v>0.19958202716823406</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="15">
       <c r="A11" s="1"/>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="15">
+      <c r="C11" s="13">
         <v>104</v>
       </c>
-      <c r="D11" s="11">
+      <c r="D11" s="9">
         <f t="shared" si="0"/>
         <v>0.16326530612244897</v>
       </c>
-      <c r="E11" s="15">
+      <c r="E11" s="13">
         <v>40</v>
       </c>
-      <c r="F11" s="11">
+      <c r="F11" s="9">
         <f t="shared" si="1"/>
         <v>0.14760147601476015</v>
       </c>
-      <c r="G11" s="15">
+      <c r="G11" s="13">
         <v>4</v>
       </c>
-      <c r="H11" s="11">
+      <c r="H11" s="9">
         <f t="shared" si="2"/>
         <v>0.13793103448275862</v>
       </c>
-      <c r="I11" s="15">
+      <c r="I11" s="13">
         <v>3</v>
       </c>
-      <c r="J11" s="12">
+      <c r="J11" s="10">
         <f t="shared" si="3"/>
         <v>0.15</v>
       </c>
@@ -1113,125 +1113,125 @@
         <f t="shared" si="4"/>
         <v>151</v>
       </c>
-      <c r="L11" s="12">
+      <c r="L11" s="10">
         <f t="shared" si="5"/>
         <v>0.15778474399164055</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="15">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="4" t="s">
         <v>15</v>
       </c>
       <c r="B12" s="1"/>
-      <c r="C12" s="16">
+      <c r="C12" s="14">
         <v>2</v>
       </c>
-      <c r="D12" s="8">
+      <c r="D12" s="6">
         <f>C12/636</f>
         <v>3.1446540880503146E-3</v>
       </c>
-      <c r="E12" s="16">
+      <c r="E12" s="14">
         <v>2</v>
       </c>
-      <c r="F12" s="8">
+      <c r="F12" s="6">
         <f t="shared" si="1"/>
         <v>7.3800738007380072E-3</v>
       </c>
-      <c r="G12" s="10">
-        <v>0</v>
-      </c>
-      <c r="H12" s="8">
+      <c r="G12" s="8">
+        <v>0</v>
+      </c>
+      <c r="H12" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I12" s="10">
-        <v>0</v>
-      </c>
-      <c r="J12" s="9">
+      <c r="I12" s="8">
+        <v>0</v>
+      </c>
+      <c r="J12" s="7">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="K12" s="10">
+      <c r="K12" s="8">
         <f t="shared" si="4"/>
         <v>4</v>
       </c>
-      <c r="L12" s="9">
-        <f>K12/954</f>
-        <v>4.1928721174004195E-3</v>
+      <c r="L12" s="7">
+        <f>K12/955</f>
+        <v>4.1884816753926706E-3</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="15">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="4" t="s">
         <v>16</v>
       </c>
       <c r="B13" s="1"/>
-      <c r="C13" s="16">
+      <c r="C13" s="14">
         <v>8</v>
       </c>
-      <c r="D13" s="8">
+      <c r="D13" s="6">
         <f>C13/636</f>
         <v>1.2578616352201259E-2</v>
       </c>
-      <c r="E13" s="16">
+      <c r="E13" s="14">
         <v>5</v>
       </c>
-      <c r="F13" s="8">
+      <c r="F13" s="6">
         <f t="shared" si="1"/>
         <v>1.8450184501845018E-2</v>
       </c>
-      <c r="G13" s="16">
+      <c r="G13" s="14">
         <v>4</v>
       </c>
-      <c r="H13" s="8">
+      <c r="H13" s="6">
         <f t="shared" si="2"/>
         <v>0.13793103448275862</v>
       </c>
-      <c r="I13" s="10">
-        <v>0</v>
-      </c>
-      <c r="J13" s="9">
+      <c r="I13" s="8">
+        <v>0</v>
+      </c>
+      <c r="J13" s="7">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="K13" s="10">
+      <c r="K13" s="8">
         <f t="shared" si="4"/>
         <v>17</v>
       </c>
-      <c r="L13" s="9">
-        <f>K13/954</f>
-        <v>1.781970649895178E-2</v>
+      <c r="L13" s="7">
+        <f>K13/955</f>
+        <v>1.7801047120418849E-2</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="15">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B14" s="1"/>
-      <c r="C14" s="10">
+      <c r="C14" s="8">
         <f>C3+C8+C12+C13</f>
         <v>637</v>
       </c>
-      <c r="D14" s="8"/>
-      <c r="E14" s="10">
+      <c r="D14" s="6"/>
+      <c r="E14" s="8">
         <f>E3+E8+E12+E13</f>
         <v>271</v>
       </c>
-      <c r="F14" s="8"/>
-      <c r="G14" s="10">
+      <c r="F14" s="6"/>
+      <c r="G14" s="8">
         <f>G3+G8+G12+G13</f>
         <v>29</v>
       </c>
-      <c r="H14" s="8"/>
-      <c r="I14" s="10">
+      <c r="H14" s="6"/>
+      <c r="I14" s="8">
         <f>I3+I8+I12+I13</f>
         <v>18</v>
       </c>
-      <c r="J14" s="9"/>
-      <c r="K14" s="10">
+      <c r="J14" s="7"/>
+      <c r="K14" s="8">
         <f t="shared" si="4"/>
         <v>955</v>
       </c>
-      <c r="L14" s="9"/>
+      <c r="L14" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -1252,7 +1252,7 @@
   <dimension ref="A1:N17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O10" sqref="O10"/>
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -1262,614 +1262,614 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15">
-      <c r="A1" s="17"/>
-      <c r="B1" s="17"/>
-      <c r="C1" s="18" t="s">
+      <c r="A1" s="15"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18" t="s">
+      <c r="D1" s="27"/>
+      <c r="E1" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18" t="s">
+      <c r="F1" s="27"/>
+      <c r="G1" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18" t="s">
+      <c r="H1" s="27"/>
+      <c r="I1" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="J1" s="18"/>
-      <c r="K1" s="18" t="s">
+      <c r="J1" s="27"/>
+      <c r="K1" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="L1" s="18"/>
-      <c r="M1" s="19"/>
-      <c r="N1" s="19"/>
+      <c r="L1" s="27"/>
+      <c r="M1" s="17"/>
+      <c r="N1" s="17"/>
     </row>
     <row r="2" spans="1:14" ht="15">
-      <c r="A2" s="17"/>
-      <c r="B2" s="17"/>
-      <c r="C2" s="20" t="s">
+      <c r="A2" s="15"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="20" t="s">
+      <c r="D2" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="E2" s="20" t="s">
+      <c r="E2" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="F2" s="20" t="s">
+      <c r="F2" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="G2" s="20" t="s">
+      <c r="G2" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="H2" s="20" t="s">
+      <c r="H2" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="I2" s="20" t="s">
+      <c r="I2" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="J2" s="20" t="s">
+      <c r="J2" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="K2" s="20" t="s">
+      <c r="K2" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="L2" s="20" t="s">
+      <c r="L2" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="M2" s="19"/>
-      <c r="N2" s="19"/>
+      <c r="M2" s="17"/>
+      <c r="N2" s="17"/>
     </row>
     <row r="3" spans="1:14" ht="15">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="17"/>
-      <c r="C3" s="21">
+      <c r="B3" s="15"/>
+      <c r="C3" s="18">
         <f>C4+C5+C6+C7</f>
         <v>151</v>
       </c>
-      <c r="D3" s="27">
+      <c r="D3" s="24">
         <f>C3/K3</f>
         <v>0.6088709677419355</v>
       </c>
-      <c r="E3" s="21">
-        <f t="shared" ref="D3:L3" si="0">E4+E5+E6+E7</f>
+      <c r="E3" s="18">
+        <f t="shared" ref="E3:K3" si="0">E4+E5+E6+E7</f>
         <v>61</v>
       </c>
-      <c r="F3" s="27">
+      <c r="F3" s="24">
         <f>E3/K3</f>
         <v>0.24596774193548387</v>
       </c>
-      <c r="G3" s="21">
+      <c r="G3" s="18">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="H3" s="27">
+      <c r="H3" s="24">
         <f>G3/K3</f>
         <v>5.2419354838709679E-2</v>
       </c>
-      <c r="I3" s="21">
+      <c r="I3" s="18">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="J3" s="27">
+      <c r="J3" s="24">
         <f>I3/K3</f>
         <v>9.2741935483870969E-2</v>
       </c>
-      <c r="K3" s="21">
+      <c r="K3" s="18">
         <f t="shared" si="0"/>
         <v>248</v>
       </c>
-      <c r="L3" s="21"/>
-      <c r="M3" s="19"/>
-      <c r="N3" s="19"/>
+      <c r="L3" s="18"/>
+      <c r="M3" s="17"/>
+      <c r="N3" s="17"/>
     </row>
     <row r="4" spans="1:14" ht="15">
-      <c r="A4" s="17"/>
-      <c r="B4" s="17" t="s">
+      <c r="A4" s="15"/>
+      <c r="B4" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="24">
-        <v>61</v>
-      </c>
-      <c r="D4" s="23">
+      <c r="C4" s="21">
+        <v>60</v>
+      </c>
+      <c r="D4" s="20">
         <f>C4/K4</f>
-        <v>0.64893617021276595</v>
-      </c>
-      <c r="E4" s="24">
+        <v>0.64516129032258063</v>
+      </c>
+      <c r="E4" s="21">
         <v>21</v>
       </c>
-      <c r="F4" s="23">
+      <c r="F4" s="20">
         <f>E4/K4</f>
-        <v>0.22340425531914893</v>
-      </c>
-      <c r="G4" s="24">
+        <v>0.22580645161290322</v>
+      </c>
+      <c r="G4" s="21">
         <v>4</v>
       </c>
-      <c r="H4" s="23">
+      <c r="H4" s="20">
         <f>G4/K4</f>
-        <v>4.2553191489361701E-2</v>
-      </c>
-      <c r="I4" s="24">
+        <v>4.3010752688172046E-2</v>
+      </c>
+      <c r="I4" s="21">
         <v>8</v>
       </c>
-      <c r="J4" s="23">
+      <c r="J4" s="20">
         <f>I4/K4</f>
-        <v>8.5106382978723402E-2</v>
-      </c>
-      <c r="K4" s="17">
+        <v>8.6021505376344093E-2</v>
+      </c>
+      <c r="K4" s="15">
         <f>C4+E4+G4+I4</f>
-        <v>94</v>
-      </c>
-      <c r="L4" s="23"/>
-      <c r="M4" s="19"/>
-      <c r="N4" s="19"/>
+        <v>93</v>
+      </c>
+      <c r="L4" s="20"/>
+      <c r="M4" s="17"/>
+      <c r="N4" s="17"/>
     </row>
     <row r="5" spans="1:14" ht="15">
-      <c r="A5" s="17"/>
-      <c r="B5" s="17" t="s">
+      <c r="A5" s="15"/>
+      <c r="B5" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="C5" s="24">
-        <v>10</v>
-      </c>
-      <c r="D5" s="23">
+      <c r="C5" s="21">
+        <v>11</v>
+      </c>
+      <c r="D5" s="20">
         <f t="shared" ref="D5:D7" si="1">C5/K5</f>
-        <v>0.83333333333333337</v>
-      </c>
-      <c r="E5" s="24">
+        <v>0.84615384615384615</v>
+      </c>
+      <c r="E5" s="21">
         <v>2</v>
       </c>
-      <c r="F5" s="23">
+      <c r="F5" s="20">
         <f t="shared" ref="F5:F7" si="2">E5/K5</f>
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="G5" s="24">
-        <v>0</v>
-      </c>
-      <c r="H5" s="23">
+        <v>0.15384615384615385</v>
+      </c>
+      <c r="G5" s="21">
+        <v>0</v>
+      </c>
+      <c r="H5" s="20">
         <f t="shared" ref="H5:H7" si="3">G5/K5</f>
         <v>0</v>
       </c>
-      <c r="I5" s="24">
-        <v>0</v>
-      </c>
-      <c r="J5" s="23">
+      <c r="I5" s="21">
+        <v>0</v>
+      </c>
+      <c r="J5" s="20">
         <f t="shared" ref="J5:J7" si="4">I5/K5</f>
         <v>0</v>
       </c>
-      <c r="K5" s="17">
+      <c r="K5" s="15">
         <f t="shared" ref="K5:K14" si="5">C5+E5+G5+I5</f>
-        <v>12</v>
-      </c>
-      <c r="L5" s="23"/>
-      <c r="M5" s="19"/>
-      <c r="N5" s="19"/>
+        <v>13</v>
+      </c>
+      <c r="L5" s="20"/>
+      <c r="M5" s="17"/>
+      <c r="N5" s="17"/>
     </row>
     <row r="6" spans="1:14" ht="15">
-      <c r="A6" s="17"/>
-      <c r="B6" s="17" t="s">
+      <c r="A6" s="15"/>
+      <c r="B6" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="24">
+      <c r="C6" s="21">
         <v>31</v>
       </c>
-      <c r="D6" s="23">
+      <c r="D6" s="20">
         <f t="shared" si="1"/>
         <v>0.51666666666666672</v>
       </c>
-      <c r="E6" s="24">
+      <c r="E6" s="21">
         <v>17</v>
       </c>
-      <c r="F6" s="23">
+      <c r="F6" s="20">
         <f t="shared" si="2"/>
         <v>0.28333333333333333</v>
       </c>
-      <c r="G6" s="24">
+      <c r="G6" s="21">
         <v>3</v>
       </c>
-      <c r="H6" s="23">
+      <c r="H6" s="20">
         <f t="shared" si="3"/>
         <v>0.05</v>
       </c>
-      <c r="I6" s="24">
+      <c r="I6" s="21">
         <v>9</v>
       </c>
-      <c r="J6" s="23">
+      <c r="J6" s="20">
         <f t="shared" si="4"/>
         <v>0.15</v>
       </c>
-      <c r="K6" s="17">
+      <c r="K6" s="15">
         <f t="shared" si="5"/>
         <v>60</v>
       </c>
-      <c r="L6" s="23"/>
-      <c r="M6" s="19"/>
-      <c r="N6" s="19"/>
+      <c r="L6" s="20"/>
+      <c r="M6" s="17"/>
+      <c r="N6" s="17"/>
     </row>
     <row r="7" spans="1:14" ht="15">
-      <c r="A7" s="17"/>
-      <c r="B7" s="17" t="s">
+      <c r="A7" s="15"/>
+      <c r="B7" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="24">
+      <c r="C7" s="21">
         <v>49</v>
       </c>
-      <c r="D7" s="23">
+      <c r="D7" s="20">
         <f t="shared" si="1"/>
         <v>0.59756097560975607</v>
       </c>
-      <c r="E7" s="24">
+      <c r="E7" s="21">
         <v>21</v>
       </c>
-      <c r="F7" s="23">
+      <c r="F7" s="20">
         <f t="shared" si="2"/>
         <v>0.25609756097560976</v>
       </c>
-      <c r="G7" s="24">
+      <c r="G7" s="21">
         <v>6</v>
       </c>
-      <c r="H7" s="23">
+      <c r="H7" s="20">
         <f t="shared" si="3"/>
         <v>7.3170731707317069E-2</v>
       </c>
-      <c r="I7" s="24">
+      <c r="I7" s="21">
         <v>6</v>
       </c>
-      <c r="J7" s="23">
+      <c r="J7" s="20">
         <f t="shared" si="4"/>
         <v>7.3170731707317069E-2</v>
       </c>
-      <c r="K7" s="17">
+      <c r="K7" s="15">
         <f t="shared" si="5"/>
         <v>82</v>
       </c>
-      <c r="L7" s="23"/>
-      <c r="M7" s="19"/>
-      <c r="N7" s="19"/>
+      <c r="L7" s="20"/>
+      <c r="M7" s="17"/>
+      <c r="N7" s="17"/>
     </row>
     <row r="8" spans="1:14" ht="15">
-      <c r="A8" s="17" t="s">
+      <c r="A8" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="17"/>
-      <c r="C8" s="21">
+      <c r="B8" s="15"/>
+      <c r="C8" s="18">
         <f>C9+C10+C11</f>
         <v>478</v>
       </c>
-      <c r="D8" s="27">
+      <c r="D8" s="24">
         <f>C8/K8</f>
         <v>0.69679300291545188</v>
       </c>
-      <c r="E8" s="21">
-        <f t="shared" ref="D8:K8" si="6">E9+E10+E11</f>
+      <c r="E8" s="18">
+        <f t="shared" ref="E8:K8" si="6">E9+E10+E11</f>
         <v>139</v>
       </c>
-      <c r="F8" s="27">
+      <c r="F8" s="24">
         <f>E8/K8</f>
         <v>0.20262390670553937</v>
       </c>
-      <c r="G8" s="21">
+      <c r="G8" s="18">
         <f t="shared" si="6"/>
         <v>40</v>
       </c>
-      <c r="H8" s="27">
+      <c r="H8" s="24">
         <f>G8/K8</f>
         <v>5.8309037900874633E-2</v>
       </c>
-      <c r="I8" s="21">
+      <c r="I8" s="18">
         <f t="shared" si="6"/>
         <v>29</v>
       </c>
-      <c r="J8" s="27">
+      <c r="J8" s="24">
         <f>I8/K8</f>
         <v>4.2274052478134108E-2</v>
       </c>
-      <c r="K8" s="21">
+      <c r="K8" s="18">
         <f t="shared" si="6"/>
         <v>686</v>
       </c>
-      <c r="L8" s="22"/>
-      <c r="M8" s="19"/>
-      <c r="N8" s="19"/>
+      <c r="L8" s="19"/>
+      <c r="M8" s="17"/>
+      <c r="N8" s="17"/>
     </row>
     <row r="9" spans="1:14" ht="15">
-      <c r="A9" s="17"/>
-      <c r="B9" s="17" t="s">
+      <c r="A9" s="15"/>
+      <c r="B9" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="C9" s="24">
+      <c r="C9" s="21">
         <v>263</v>
       </c>
-      <c r="D9" s="23">
+      <c r="D9" s="20">
         <f>C9/K9</f>
         <v>0.76453488372093026</v>
       </c>
-      <c r="E9" s="24">
+      <c r="E9" s="21">
         <v>59</v>
       </c>
-      <c r="F9" s="23">
+      <c r="F9" s="20">
         <f>E9/K9</f>
         <v>0.17151162790697674</v>
       </c>
-      <c r="G9" s="24">
+      <c r="G9" s="21">
         <v>6</v>
       </c>
-      <c r="H9" s="23">
+      <c r="H9" s="20">
         <f>G9/K9</f>
         <v>1.7441860465116279E-2</v>
       </c>
-      <c r="I9" s="24">
+      <c r="I9" s="21">
         <v>16</v>
       </c>
-      <c r="J9" s="23">
+      <c r="J9" s="20">
         <f>I9/K9</f>
         <v>4.6511627906976744E-2</v>
       </c>
-      <c r="K9" s="17">
+      <c r="K9" s="15">
         <f t="shared" si="5"/>
         <v>344</v>
       </c>
-      <c r="L9" s="23"/>
-      <c r="M9" s="19"/>
-      <c r="N9" s="19"/>
+      <c r="L9" s="20"/>
+      <c r="M9" s="17"/>
+      <c r="N9" s="17"/>
     </row>
     <row r="10" spans="1:14" ht="15">
-      <c r="A10" s="17"/>
-      <c r="B10" s="17" t="s">
+      <c r="A10" s="15"/>
+      <c r="B10" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="24">
+      <c r="C10" s="21">
         <v>151</v>
       </c>
-      <c r="D10" s="23">
+      <c r="D10" s="20">
         <f t="shared" ref="D10:D11" si="7">C10/K10</f>
         <v>0.79057591623036649</v>
       </c>
-      <c r="E10" s="24">
+      <c r="E10" s="21">
         <v>25</v>
       </c>
-      <c r="F10" s="23">
+      <c r="F10" s="20">
         <f t="shared" ref="F10:F11" si="8">E10/K10</f>
         <v>0.13089005235602094</v>
       </c>
-      <c r="G10" s="24">
+      <c r="G10" s="21">
         <v>11</v>
       </c>
-      <c r="H10" s="23">
+      <c r="H10" s="20">
         <f t="shared" ref="H10:H11" si="9">G10/K10</f>
         <v>5.7591623036649213E-2</v>
       </c>
-      <c r="I10" s="24">
+      <c r="I10" s="21">
         <v>4</v>
       </c>
-      <c r="J10" s="23">
+      <c r="J10" s="20">
         <f t="shared" ref="J10:J11" si="10">I10/K10</f>
         <v>2.0942408376963352E-2</v>
       </c>
-      <c r="K10" s="17">
+      <c r="K10" s="15">
         <f t="shared" si="5"/>
         <v>191</v>
       </c>
-      <c r="L10" s="23"/>
-      <c r="M10" s="19"/>
-      <c r="N10" s="19"/>
+      <c r="L10" s="20"/>
+      <c r="M10" s="17"/>
+      <c r="N10" s="17"/>
     </row>
     <row r="11" spans="1:14" ht="15">
-      <c r="A11" s="17"/>
-      <c r="B11" s="17" t="s">
+      <c r="A11" s="15"/>
+      <c r="B11" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="24">
+      <c r="C11" s="21">
         <v>64</v>
       </c>
-      <c r="D11" s="23">
+      <c r="D11" s="20">
         <f t="shared" si="7"/>
         <v>0.42384105960264901</v>
       </c>
-      <c r="E11" s="24">
+      <c r="E11" s="21">
         <v>55</v>
       </c>
-      <c r="F11" s="23">
+      <c r="F11" s="20">
         <f t="shared" si="8"/>
         <v>0.36423841059602646</v>
       </c>
-      <c r="G11" s="24">
+      <c r="G11" s="21">
         <v>23</v>
       </c>
-      <c r="H11" s="23">
+      <c r="H11" s="20">
         <f t="shared" si="9"/>
         <v>0.15231788079470199</v>
       </c>
-      <c r="I11" s="24">
+      <c r="I11" s="21">
         <v>9</v>
       </c>
-      <c r="J11" s="23">
+      <c r="J11" s="20">
         <f t="shared" si="10"/>
         <v>5.9602649006622516E-2</v>
       </c>
-      <c r="K11" s="17">
+      <c r="K11" s="15">
         <f t="shared" si="5"/>
         <v>151</v>
       </c>
-      <c r="L11" s="23"/>
-      <c r="M11" s="19"/>
-      <c r="N11" s="19"/>
+      <c r="L11" s="20"/>
+      <c r="M11" s="17"/>
+      <c r="N11" s="17"/>
     </row>
     <row r="12" spans="1:14" ht="15">
-      <c r="A12" s="17" t="s">
+      <c r="A12" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="B12" s="17"/>
-      <c r="C12" s="25">
-        <v>0</v>
-      </c>
-      <c r="D12" s="26">
+      <c r="B12" s="15"/>
+      <c r="C12" s="22">
+        <v>0</v>
+      </c>
+      <c r="D12" s="23">
         <f>C12/K12</f>
         <v>0</v>
       </c>
-      <c r="E12" s="25">
+      <c r="E12" s="22">
         <v>3</v>
       </c>
-      <c r="F12" s="26">
+      <c r="F12" s="23">
         <f>E12/K12</f>
         <v>0.75</v>
       </c>
-      <c r="G12" s="25">
-        <v>0</v>
-      </c>
-      <c r="H12" s="26">
+      <c r="G12" s="22">
+        <v>0</v>
+      </c>
+      <c r="H12" s="23">
         <f>G12/K12</f>
         <v>0</v>
       </c>
-      <c r="I12" s="25">
+      <c r="I12" s="22">
         <v>1</v>
       </c>
-      <c r="J12" s="26">
+      <c r="J12" s="23">
         <f>I12/K12</f>
         <v>0.25</v>
       </c>
-      <c r="K12" s="21">
+      <c r="K12" s="18">
         <f t="shared" si="5"/>
         <v>4</v>
       </c>
-      <c r="L12" s="22"/>
-      <c r="M12" s="19"/>
-      <c r="N12" s="19"/>
+      <c r="L12" s="19"/>
+      <c r="M12" s="17"/>
+      <c r="N12" s="17"/>
     </row>
     <row r="13" spans="1:14" ht="15">
-      <c r="A13" s="17" t="s">
+      <c r="A13" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="B13" s="17"/>
-      <c r="C13" s="25">
+      <c r="B13" s="15"/>
+      <c r="C13" s="22">
         <v>8</v>
       </c>
-      <c r="D13" s="26">
+      <c r="D13" s="23">
         <f t="shared" ref="D13:D14" si="11">C13/K13</f>
         <v>0.47058823529411764</v>
       </c>
-      <c r="E13" s="25">
+      <c r="E13" s="22">
         <v>6</v>
       </c>
-      <c r="F13" s="26">
+      <c r="F13" s="23">
         <f t="shared" ref="F13:F14" si="12">E13/K13</f>
         <v>0.35294117647058826</v>
       </c>
-      <c r="G13" s="25">
-        <v>0</v>
-      </c>
-      <c r="H13" s="26">
+      <c r="G13" s="22">
+        <v>0</v>
+      </c>
+      <c r="H13" s="23">
         <f t="shared" ref="H13:H14" si="13">G13/K13</f>
         <v>0</v>
       </c>
-      <c r="I13" s="25">
+      <c r="I13" s="22">
         <v>3</v>
       </c>
-      <c r="J13" s="26">
+      <c r="J13" s="23">
         <f t="shared" ref="J13:J14" si="14">I13/K13</f>
         <v>0.17647058823529413</v>
       </c>
-      <c r="K13" s="21">
+      <c r="K13" s="18">
         <f t="shared" si="5"/>
         <v>17</v>
       </c>
-      <c r="L13" s="22"/>
-      <c r="M13" s="19"/>
-      <c r="N13" s="19"/>
+      <c r="L13" s="19"/>
+      <c r="M13" s="17"/>
+      <c r="N13" s="17"/>
     </row>
     <row r="14" spans="1:14" ht="15">
-      <c r="A14" s="17" t="s">
+      <c r="A14" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="17"/>
-      <c r="C14" s="21">
+      <c r="B14" s="15"/>
+      <c r="C14" s="18">
         <v>637</v>
       </c>
-      <c r="D14" s="26">
+      <c r="D14" s="23">
         <f t="shared" si="11"/>
         <v>0.66701570680628275</v>
       </c>
-      <c r="E14" s="21">
+      <c r="E14" s="18">
         <v>209</v>
       </c>
-      <c r="F14" s="26">
+      <c r="F14" s="23">
         <f t="shared" si="12"/>
         <v>0.218848167539267</v>
       </c>
-      <c r="G14" s="21">
+      <c r="G14" s="18">
         <v>53</v>
       </c>
-      <c r="H14" s="26">
+      <c r="H14" s="23">
         <f t="shared" si="13"/>
         <v>5.549738219895288E-2</v>
       </c>
-      <c r="I14" s="21">
+      <c r="I14" s="18">
         <v>56</v>
       </c>
-      <c r="J14" s="26">
+      <c r="J14" s="23">
         <f t="shared" si="14"/>
         <v>5.8638743455497383E-2</v>
       </c>
-      <c r="K14" s="21">
+      <c r="K14" s="18">
         <f t="shared" si="5"/>
         <v>955</v>
       </c>
-      <c r="L14" s="22"/>
-      <c r="M14" s="19"/>
-      <c r="N14" s="19"/>
+      <c r="L14" s="19"/>
+      <c r="M14" s="17"/>
+      <c r="N14" s="17"/>
     </row>
     <row r="15" spans="1:14">
-      <c r="A15" s="19"/>
-      <c r="B15" s="19"/>
-      <c r="C15" s="19"/>
-      <c r="D15" s="19"/>
-      <c r="E15" s="19"/>
-      <c r="F15" s="19"/>
-      <c r="G15" s="19"/>
-      <c r="H15" s="19"/>
-      <c r="I15" s="19"/>
-      <c r="J15" s="19"/>
-      <c r="K15" s="19"/>
-      <c r="L15" s="19"/>
-      <c r="M15" s="19"/>
-      <c r="N15" s="19"/>
+      <c r="A15" s="17"/>
+      <c r="B15" s="17"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="17"/>
+      <c r="F15" s="17"/>
+      <c r="G15" s="17"/>
+      <c r="H15" s="17"/>
+      <c r="I15" s="17"/>
+      <c r="J15" s="17"/>
+      <c r="K15" s="17"/>
+      <c r="L15" s="17"/>
+      <c r="M15" s="17"/>
+      <c r="N15" s="17"/>
     </row>
     <row r="16" spans="1:14">
-      <c r="A16" s="19"/>
-      <c r="B16" s="19"/>
-      <c r="C16" s="19"/>
-      <c r="D16" s="19"/>
-      <c r="E16" s="19"/>
-      <c r="F16" s="19"/>
-      <c r="G16" s="19"/>
-      <c r="H16" s="19"/>
-      <c r="I16" s="19"/>
-      <c r="J16" s="19"/>
-      <c r="K16" s="19"/>
-      <c r="L16" s="19"/>
-      <c r="M16" s="19"/>
-      <c r="N16" s="19"/>
+      <c r="A16" s="17"/>
+      <c r="B16" s="17"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="17"/>
+      <c r="G16" s="17"/>
+      <c r="H16" s="17"/>
+      <c r="I16" s="17"/>
+      <c r="J16" s="17"/>
+      <c r="K16" s="17"/>
+      <c r="L16" s="17"/>
+      <c r="M16" s="17"/>
+      <c r="N16" s="17"/>
     </row>
     <row r="17" spans="1:14">
-      <c r="A17" s="19"/>
-      <c r="B17" s="19"/>
-      <c r="C17" s="19"/>
-      <c r="D17" s="19"/>
-      <c r="E17" s="19"/>
-      <c r="F17" s="19"/>
-      <c r="G17" s="19"/>
-      <c r="H17" s="19"/>
-      <c r="I17" s="19"/>
-      <c r="J17" s="19"/>
-      <c r="K17" s="19"/>
-      <c r="L17" s="19"/>
-      <c r="M17" s="19"/>
-      <c r="N17" s="19"/>
+      <c r="A17" s="17"/>
+      <c r="B17" s="17"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="17"/>
+      <c r="G17" s="17"/>
+      <c r="H17" s="17"/>
+      <c r="I17" s="17"/>
+      <c r="J17" s="17"/>
+      <c r="K17" s="17"/>
+      <c r="L17" s="17"/>
+      <c r="M17" s="17"/>
+      <c r="N17" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>